<commit_message>
entered growth data, created growth assignment
</commit_message>
<xml_diff>
--- a/density_2025.xlsx
+++ b/density_2025.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maryo/GitHub/biol 402/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maryo/GitHub/biol_402/Biol_402_2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E2A956-20CF-CD4E-8496-29BADD4318AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84757D50-ED98-FF4E-A330-8C315E9EF4AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="980" windowWidth="27640" windowHeight="15600" xr2:uid="{01EB99D4-2C2B-A441-AB8B-58EA3D90905E}"/>
+    <workbookView xWindow="780" yWindow="720" windowWidth="27640" windowHeight="15600" xr2:uid="{01EB99D4-2C2B-A441-AB8B-58EA3D90905E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="18">
   <si>
     <t>plot</t>
   </si>
@@ -64,12 +64,6 @@
     <t>sept_5_density_exp</t>
   </si>
   <si>
-    <t>sept_6_density1</t>
-  </si>
-  <si>
-    <t>sept_6_densityF</t>
-  </si>
-  <si>
     <t>sept_6_quadrat</t>
   </si>
   <si>
@@ -92,6 +86,9 @@
   </si>
   <si>
     <t>sept_16_zj</t>
+  </si>
+  <si>
+    <t>sept_6_density</t>
   </si>
 </sst>
 </file>
@@ -450,15 +447,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F10F89A-1874-0B4D-BB14-BB1AB0B64851}">
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:O25"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -475,37 +475,34 @@
         <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -525,34 +522,31 @@
         <v>29</v>
       </c>
       <c r="G2" s="1">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="H2" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I2" s="1">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="J2" s="1">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="K2" s="1">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="L2" s="1">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="M2" s="1">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="N2" s="1">
-        <v>11</v>
-      </c>
-      <c r="O2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -572,34 +566,31 @@
         <v>56</v>
       </c>
       <c r="G3" s="1">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="H3" s="1">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" s="1">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="K3" s="1">
-        <v>12</v>
+        <v>97</v>
       </c>
       <c r="L3" s="1">
-        <v>97</v>
+        <v>0</v>
       </c>
       <c r="M3" s="1">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="N3" s="1">
-        <v>45</v>
-      </c>
-      <c r="O3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -619,34 +610,31 @@
         <v>111</v>
       </c>
       <c r="G4" s="1">
-        <v>111</v>
+        <v>33</v>
       </c>
       <c r="H4" s="1">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="I4" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J4" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K4" s="1">
-        <v>5</v>
+        <v>163</v>
       </c>
       <c r="L4" s="1">
-        <v>163</v>
+        <v>0</v>
       </c>
       <c r="M4" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N4" s="1">
-        <v>8</v>
-      </c>
-      <c r="O4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -666,34 +654,31 @@
         <v>48</v>
       </c>
       <c r="G5" s="1">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="H5" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="I5" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J5" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="K5" s="1">
+        <v>70</v>
+      </c>
+      <c r="L5" s="1">
         <v>10</v>
       </c>
-      <c r="L5" s="1">
-        <v>70</v>
-      </c>
       <c r="M5" s="1">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="N5" s="1">
-        <v>40</v>
-      </c>
-      <c r="O5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -713,34 +698,31 @@
         <v>101</v>
       </c>
       <c r="G6" s="1">
-        <v>101</v>
+        <v>25</v>
       </c>
       <c r="H6" s="1">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="I6" s="1">
         <v>0</v>
       </c>
       <c r="J6" s="1">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="K6" s="1">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="L6" s="1">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="M6" s="1">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="N6" s="1">
-        <v>50</v>
-      </c>
-      <c r="O6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -757,37 +739,34 @@
         <v>90</v>
       </c>
       <c r="F7" s="1">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G7" s="1">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="H7" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="I7" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J7" s="1">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="K7" s="1">
-        <v>16</v>
+        <v>132</v>
       </c>
       <c r="L7" s="1">
-        <v>132</v>
+        <v>0</v>
       </c>
       <c r="M7" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N7" s="1">
-        <v>5</v>
-      </c>
-      <c r="O7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -807,34 +786,31 @@
         <v>65</v>
       </c>
       <c r="G8" s="1">
-        <v>65</v>
+        <v>13</v>
       </c>
       <c r="H8" s="1">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="I8" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J8" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="K8" s="1">
+        <v>52</v>
+      </c>
+      <c r="L8" s="1">
         <v>10</v>
       </c>
-      <c r="L8" s="1">
-        <v>52</v>
-      </c>
       <c r="M8" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="N8" s="1">
-        <v>20</v>
-      </c>
-      <c r="O8" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -851,37 +827,34 @@
         <v>50</v>
       </c>
       <c r="F9" s="1">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="G9" s="1">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="H9" s="1">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="I9" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="J9" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="K9" s="1">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="L9" s="1">
-        <v>56</v>
+        <v>6</v>
       </c>
       <c r="M9" s="1">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="N9" s="1">
-        <v>15</v>
-      </c>
-      <c r="O9" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -901,34 +874,31 @@
         <v>24</v>
       </c>
       <c r="G10" s="1">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="H10" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="I10" s="1">
         <v>0</v>
       </c>
       <c r="J10" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K10" s="1">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="L10" s="1">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="M10" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N10" s="1">
-        <v>3</v>
-      </c>
-      <c r="O10" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -948,34 +918,31 @@
         <v>101</v>
       </c>
       <c r="G11" s="1">
-        <v>101</v>
+        <v>27</v>
       </c>
       <c r="H11" s="1">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="I11" s="1">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="J11" s="1">
         <v>15</v>
       </c>
       <c r="K11" s="1">
-        <v>15</v>
+        <v>86</v>
       </c>
       <c r="L11" s="1">
-        <v>86</v>
+        <v>20</v>
       </c>
       <c r="M11" s="1">
         <v>20</v>
       </c>
       <c r="N11" s="1">
-        <v>20</v>
-      </c>
-      <c r="O11" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -995,34 +962,31 @@
         <v>77</v>
       </c>
       <c r="G12" s="1">
-        <v>77</v>
+        <v>18</v>
       </c>
       <c r="H12" s="1">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="I12" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J12" s="1">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="K12" s="1">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="L12" s="1">
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="M12" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="N12" s="1">
-        <v>10</v>
-      </c>
-      <c r="O12" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1042,34 +1006,31 @@
         <v>78</v>
       </c>
       <c r="G13" s="1">
-        <v>78</v>
+        <v>29</v>
       </c>
       <c r="H13" s="1">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="I13" s="1">
         <v>0</v>
       </c>
       <c r="J13" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K13" s="1">
-        <v>6</v>
+        <v>119</v>
       </c>
       <c r="L13" s="1">
-        <v>119</v>
+        <v>0</v>
       </c>
       <c r="M13" s="1">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="N13" s="1">
-        <v>50</v>
-      </c>
-      <c r="O13" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1090,21 +1051,20 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
+      <c r="K14" s="1">
+        <v>57</v>
+      </c>
       <c r="L14" s="1">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="M14" s="1">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="N14" s="1">
-        <v>18</v>
-      </c>
-      <c r="O14" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1124,22 +1084,22 @@
         <v>112</v>
       </c>
       <c r="G15" s="1">
-        <v>112</v>
+        <v>43</v>
       </c>
       <c r="H15" s="1">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="I15" s="1">
         <v>0</v>
       </c>
       <c r="J15" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K15" s="1">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="L15" s="1">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="M15" s="1">
         <v>0</v>
@@ -1147,11 +1107,8 @@
       <c r="N15" s="1">
         <v>0</v>
       </c>
-      <c r="O15" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1171,22 +1128,22 @@
         <v>54</v>
       </c>
       <c r="G16" s="1">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="H16" s="1">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="I16" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J16" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K16" s="1">
-        <v>2</v>
+        <v>68</v>
       </c>
       <c r="L16" s="1">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="M16" s="1">
         <v>0</v>
@@ -1194,11 +1151,8 @@
       <c r="N16" s="1">
         <v>0</v>
       </c>
-      <c r="O16" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1218,10 +1172,10 @@
         <v>52</v>
       </c>
       <c r="G17" s="1">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="H17" s="1">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I17" s="1">
         <v>0</v>
@@ -1230,22 +1184,19 @@
         <v>0</v>
       </c>
       <c r="K17" s="1">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="L17" s="1">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="M17" s="1">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="N17" s="1">
-        <v>20</v>
-      </c>
-      <c r="O17" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1266,21 +1217,20 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
+      <c r="K18" s="1">
+        <v>45</v>
+      </c>
       <c r="L18" s="1">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="M18" s="1">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="N18" s="1">
-        <v>20</v>
-      </c>
-      <c r="O18" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1300,34 +1250,31 @@
         <v>101</v>
       </c>
       <c r="G19" s="1">
-        <v>101</v>
+        <v>27</v>
       </c>
       <c r="H19" s="1">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="I19" s="1">
         <v>0</v>
       </c>
       <c r="J19" s="1">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="K19" s="1">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="L19" s="1">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="M19" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N19" s="1">
-        <v>6</v>
-      </c>
-      <c r="O19" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1347,34 +1294,31 @@
         <v>26</v>
       </c>
       <c r="G20" s="1">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="H20" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="I20" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J20" s="1">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="K20" s="1">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="L20" s="1">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="M20" s="1">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="N20" s="1">
-        <v>40</v>
-      </c>
-      <c r="O20" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1394,10 +1338,10 @@
         <v>48</v>
       </c>
       <c r="G21" s="1">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="H21" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="I21" s="1">
         <v>0</v>
@@ -1406,22 +1350,19 @@
         <v>0</v>
       </c>
       <c r="K21" s="1">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="L21" s="1">
-        <v>71</v>
+        <v>0.1</v>
       </c>
       <c r="M21" s="1">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="N21" s="1">
-        <v>1</v>
-      </c>
-      <c r="O21" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1441,34 +1382,31 @@
         <v>38</v>
       </c>
       <c r="G22" s="1">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="H22" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I22" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K22" s="1">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="L22" s="1">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="M22" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N22" s="1">
-        <v>3</v>
-      </c>
-      <c r="O22" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1488,34 +1426,31 @@
         <v>53</v>
       </c>
       <c r="G23" s="1">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="H23" s="1">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I23" s="1">
         <v>0</v>
       </c>
       <c r="J23" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K23" s="1">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="L23" s="1">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="M23" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N23" s="1">
-        <v>8</v>
-      </c>
-      <c r="O23" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1535,34 +1470,31 @@
         <v>45</v>
       </c>
       <c r="G24" s="1">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="H24" s="1">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="I24" s="1">
         <v>0</v>
       </c>
       <c r="J24" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K24" s="1">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="L24" s="1">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="M24" s="1">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="N24" s="1">
-        <v>50</v>
-      </c>
-      <c r="O24" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1582,10 +1514,10 @@
         <v>54</v>
       </c>
       <c r="G25" s="1">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="H25" s="1">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="I25" s="1">
         <v>0</v>
@@ -1594,18 +1526,15 @@
         <v>0</v>
       </c>
       <c r="K25" s="1">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="L25" s="1">
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="M25" s="1">
         <v>0</v>
       </c>
       <c r="N25" s="1">
-        <v>0</v>
-      </c>
-      <c r="O25" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>